<commit_message>
feat：open tuteng and running
</commit_message>
<xml_diff>
--- a/Excels/Global_全局表.xlsx
+++ b/Excels/Global_全局表.xlsx
@@ -212,7 +212,7 @@
     <t>8855.69|94653.50|1753.76</t>
   </si>
   <si>
-    <t>9000.84|94675.87|1823.51</t>
+    <t>12714.94|94634.66|1958.03</t>
   </si>
   <si>
     <t>RG_Back_Loc</t>
@@ -224,7 +224,7 @@
     <t>13641.69|94653.50|1753.76</t>
   </si>
   <si>
-    <t>12714.94|94634.66|1958.03</t>
+    <t>13774.98|94678.81|1790</t>
   </si>
   <si>
     <t>RG_FOV_VALUE</t>
@@ -1515,7 +1515,7 @@
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="O21" sqref="O21"/>
+      <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8166666666667" defaultRowHeight="16.5"/>

</xml_diff>